<commit_message>
File Multilingual Continuous Job.xlsx committed.
</commit_message>
<xml_diff>
--- a/cs-de-es/Multilingual Continuous Job-en-cs-de-es-T-C.xlsx
+++ b/cs-de-es/Multilingual Continuous Job-en-cs-de-es-T-C.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\AppData\Roaming\memsource\mso-converter\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CED450C-FF6D-44AF-835A-C2A65831FCF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7DF72942-A615-4474-934C-A8BE61F40363}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="15750" windowHeight="11055"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21240" windowHeight="10815"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>

</xml_diff>